<commit_message>
Got the colored letters to work
yeah!!! It was not easy to have multiple colored letters in one line.
</commit_message>
<xml_diff>
--- a/PartialTrialDIR/PartialTrial1.xlsx
+++ b/PartialTrialDIR/PartialTrial1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19780" windowHeight="8500" tabRatio="500"/>
+    <workbookView xWindow="120" yWindow="2520" windowWidth="19780" windowHeight="8500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>StimSet</t>
   </si>
@@ -60,22 +60,13 @@
     <t>RespDur</t>
   </si>
   <si>
-    <t>A B C D E F</t>
-  </si>
-  <si>
-    <t>UpBrack</t>
-  </si>
-  <si>
-    <t>G H J K M T</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [   ] </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [                ]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">              [      ]</t>
+    <t>ABXD{EF}</t>
+  </si>
+  <si>
+    <t>{ABYDEF}</t>
+  </si>
+  <si>
+    <t>A{BZDE}F</t>
   </si>
 </sst>
 </file>
@@ -135,8 +126,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -476,163 +468,150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>C2+B2</f>
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <f>B2+C2+D2</f>
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <f>D2+I2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <f>C3+B3</f>
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H4" si="0">B3+C3+D3</f>
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" t="s">
-        <v>12</v>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J4" si="1">D3+I3</f>
+        <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <f>D2+C2</f>
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <f>C2+D2+E2</f>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f>C4+B4</f>
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4">
         <v>2</v>
       </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <f>E2+J2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <f>D3+C3</f>
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I4" si="0">C3+D3+E3</f>
-        <v>2</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K4" si="1">E3+J3</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <f>D4+C4</f>
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>6</v>
-      </c>
       <c r="H4">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>

</xml_diff>